<commit_message>
Updated budget viz code
</commit_message>
<xml_diff>
--- a/Budget data/Berkeley Budget.xlsx
+++ b/Budget data/Berkeley Budget.xlsx
@@ -1286,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q107"/>
+  <dimension ref="A1:H172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1301,7 +1301,7 @@
     <col min="16" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1326,32 +1326,8 @@
       <c r="H1" t="s">
         <v>110</v>
       </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1376,16 +1352,8 @@
       <c r="H2">
         <v>50768165</v>
       </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1410,32 +1378,8 @@
       <c r="H3">
         <v>12500000</v>
       </c>
-      <c r="J3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="1">
-        <v>984051</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1032227</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1052122</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1070929</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1092347</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1209625</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>1233817</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1460,32 +1404,8 @@
       <c r="H4">
         <v>2809200</v>
       </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="1">
-        <v>3110933</v>
-      </c>
-      <c r="L4" s="1">
-        <v>3226626</v>
-      </c>
-      <c r="M4" s="1">
-        <v>2844356</v>
-      </c>
-      <c r="N4" s="1">
-        <v>3050030</v>
-      </c>
-      <c r="O4" s="1">
-        <v>3191390</v>
-      </c>
-      <c r="P4" s="1">
-        <v>3417084</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>3475415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1510,32 +1430,8 @@
       <c r="H5">
         <v>18522000</v>
       </c>
-      <c r="J5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="1">
-        <v>9542084</v>
-      </c>
-      <c r="L5" s="1">
-        <v>9762684</v>
-      </c>
-      <c r="M5" s="1">
-        <v>9948439</v>
-      </c>
-      <c r="N5" s="1">
-        <v>11826449</v>
-      </c>
-      <c r="O5" s="1">
-        <v>12027328</v>
-      </c>
-      <c r="P5" s="1">
-        <v>12816390</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>13081657</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1560,32 +1456,8 @@
       <c r="H6">
         <v>18727959</v>
       </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="1">
-        <v>969769</v>
-      </c>
-      <c r="L6" s="1">
-        <v>947947</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1005000</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1005000</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1005000</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1250000</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1250000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1610,32 +1482,8 @@
       <c r="H7">
         <v>8089178</v>
       </c>
-      <c r="J7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="1">
-        <v>3917791</v>
-      </c>
-      <c r="L7" s="1">
-        <v>4130013</v>
-      </c>
-      <c r="M7" s="1">
-        <v>4186198</v>
-      </c>
-      <c r="N7" s="1">
-        <v>4256305</v>
-      </c>
-      <c r="O7" s="1">
-        <v>4341432</v>
-      </c>
-      <c r="P7" s="1">
-        <v>4812892</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>4909150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1660,32 +1508,8 @@
       <c r="H8">
         <v>14496610</v>
       </c>
-      <c r="J8" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="1">
-        <v>2052466</v>
-      </c>
-      <c r="L8" s="1">
-        <v>2065845</v>
-      </c>
-      <c r="M8" s="1">
-        <v>2023244</v>
-      </c>
-      <c r="N8" s="1">
-        <v>1866961</v>
-      </c>
-      <c r="O8" s="1">
-        <v>1866961</v>
-      </c>
-      <c r="P8" s="1">
-        <v>1352432</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>1410489</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1710,32 +1534,8 @@
       <c r="H9">
         <v>10475208</v>
       </c>
-      <c r="J9" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="1">
-        <v>52888</v>
-      </c>
-      <c r="L9" s="1">
-        <v>28164</v>
-      </c>
-      <c r="M9" s="1">
-        <v>35000</v>
-      </c>
-      <c r="N9" s="1">
-        <v>35000</v>
-      </c>
-      <c r="O9" s="1">
-        <v>35000</v>
-      </c>
-      <c r="P9" s="1">
-        <v>35000</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1760,32 +1560,8 @@
       <c r="H10">
         <v>6600871</v>
       </c>
-      <c r="J10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="1">
-        <v>4613</v>
-      </c>
-      <c r="L10" s="1">
-        <v>10</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1810,32 +1586,8 @@
       <c r="H11">
         <v>243367</v>
       </c>
-      <c r="J11" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="1">
-        <v>226933</v>
-      </c>
-      <c r="L11" s="1">
-        <v>226450</v>
-      </c>
-      <c r="M11" s="1">
-        <v>263000</v>
-      </c>
-      <c r="N11" s="1">
-        <v>263000</v>
-      </c>
-      <c r="O11" s="1">
-        <v>263000</v>
-      </c>
-      <c r="P11" s="1">
-        <v>489000</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>489000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1860,32 +1612,8 @@
       <c r="H12">
         <v>2244165</v>
       </c>
-      <c r="J12" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" s="1">
-        <v>165672</v>
-      </c>
-      <c r="L12" s="1">
-        <v>164558</v>
-      </c>
-      <c r="M12" s="1">
-        <v>168550</v>
-      </c>
-      <c r="N12" s="1">
-        <v>168550</v>
-      </c>
-      <c r="O12" s="1">
-        <v>168550</v>
-      </c>
-      <c r="P12" s="1">
-        <v>174011</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>174011</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1912,32 +1640,8 @@
         <f>4913194 + 1984644</f>
         <v>6897838</v>
       </c>
-      <c r="J13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1">
-        <v>488864</v>
-      </c>
-      <c r="M13" s="1">
-        <v>496424</v>
-      </c>
-      <c r="N13" s="1">
-        <v>546823</v>
-      </c>
-      <c r="O13" s="1">
-        <v>557759</v>
-      </c>
-      <c r="P13" s="1">
-        <v>664136</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>674098</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1964,32 +1668,8 @@
         <f>SUM(H2:H13)</f>
         <v>152374561</v>
       </c>
-      <c r="J14" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0</v>
-      </c>
-      <c r="M14" s="1">
-        <v>30000</v>
-      </c>
-      <c r="N14" s="1">
-        <v>30000</v>
-      </c>
-      <c r="O14" s="1">
-        <v>30000</v>
-      </c>
-      <c r="P14" s="1">
-        <v>30000</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2014,34 +1694,8 @@
       <c r="H15">
         <v>11114390</v>
       </c>
-      <c r="J15" t="s">
-        <v>104</v>
-      </c>
-      <c r="K15" s="1">
-        <v>21027200</v>
-      </c>
-      <c r="L15" s="1">
-        <v>22073388</v>
-      </c>
-      <c r="M15" s="1">
-        <v>22052333</v>
-      </c>
-      <c r="N15" s="1">
-        <v>24119047</v>
-      </c>
-      <c r="O15" s="1">
-        <v>24578767</v>
-      </c>
-      <c r="P15" s="1">
-        <f>SUM(P3:P14)</f>
-        <v>26250570</v>
-      </c>
-      <c r="Q15" s="1">
-        <f>SUM(Q3:Q14)</f>
-        <v>26762637</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2069,49 +1723,8 @@
         <f>SUM(H15,H2:H13)</f>
         <v>163488951</v>
       </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J18" t="s">
-        <v>55</v>
-      </c>
-      <c r="K18" s="1">
-        <v>33861186</v>
-      </c>
-      <c r="L18" s="1">
-        <v>34101574</v>
-      </c>
-      <c r="M18" s="1">
-        <v>36673523</v>
-      </c>
-      <c r="N18" s="1">
-        <v>37600783</v>
-      </c>
-      <c r="O18" s="1">
-        <v>37710238</v>
-      </c>
-      <c r="P18" s="1">
-        <v>40453300</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>41242753</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2136,32 +1749,8 @@
       <c r="H19" t="s">
         <v>110</v>
       </c>
-      <c r="J19" t="s">
-        <v>56</v>
-      </c>
-      <c r="K19" s="1">
-        <v>5230735</v>
-      </c>
-      <c r="L19" s="1">
-        <v>5478724</v>
-      </c>
-      <c r="M19" s="1">
-        <v>5558716</v>
-      </c>
-      <c r="N19" s="1">
-        <v>5311066</v>
-      </c>
-      <c r="O19" s="1">
-        <v>5311066</v>
-      </c>
-      <c r="P19" s="1">
-        <v>6245459</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>6270459</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2186,32 +1775,8 @@
       <c r="H20">
         <v>2074738</v>
       </c>
-      <c r="J20" t="s">
-        <v>57</v>
-      </c>
-      <c r="K20" s="1">
-        <v>13315067</v>
-      </c>
-      <c r="L20" s="1">
-        <v>13588024</v>
-      </c>
-      <c r="M20" s="1">
-        <v>12801227</v>
-      </c>
-      <c r="N20" s="1">
-        <v>12801227</v>
-      </c>
-      <c r="O20" s="1">
-        <v>12801227</v>
-      </c>
-      <c r="P20" s="1">
-        <v>21384982</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>22827768</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2236,32 +1801,8 @@
       <c r="H21">
         <v>2304413</v>
       </c>
-      <c r="J21" t="s">
-        <v>58</v>
-      </c>
-      <c r="K21" s="1">
-        <v>2467033</v>
-      </c>
-      <c r="L21" s="1">
-        <v>2316216</v>
-      </c>
-      <c r="M21" s="1">
-        <v>2365140</v>
-      </c>
-      <c r="N21" s="1">
-        <v>2502740</v>
-      </c>
-      <c r="O21" s="1">
-        <v>2510569</v>
-      </c>
-      <c r="P21" s="1">
-        <v>2388633</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>2369937</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2286,32 +1827,8 @@
       <c r="H22">
         <v>738060</v>
       </c>
-      <c r="J22" t="s">
-        <v>59</v>
-      </c>
-      <c r="K22" s="1">
-        <v>577473</v>
-      </c>
-      <c r="L22" s="1">
-        <v>245868</v>
-      </c>
-      <c r="M22" s="1">
-        <v>240501</v>
-      </c>
-      <c r="N22" s="1">
-        <v>240501</v>
-      </c>
-      <c r="O22" s="1">
-        <v>240501</v>
-      </c>
-      <c r="P22" s="1">
-        <v>240501</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>240501</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2336,32 +1853,8 @@
       <c r="H23">
         <v>6106514</v>
       </c>
-      <c r="J23" t="s">
-        <v>60</v>
-      </c>
-      <c r="K23" s="1">
-        <v>9249750</v>
-      </c>
-      <c r="L23" s="1">
-        <v>14087031</v>
-      </c>
-      <c r="M23" s="1">
-        <v>13552248</v>
-      </c>
-      <c r="N23" s="1">
-        <v>12238260</v>
-      </c>
-      <c r="O23" s="1">
-        <v>12544854</v>
-      </c>
-      <c r="P23" s="1">
-        <v>14528343</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>15003859</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -2386,32 +1879,8 @@
       <c r="H24">
         <v>2560121</v>
       </c>
-      <c r="J24" t="s">
-        <v>61</v>
-      </c>
-      <c r="K24" s="1">
-        <v>3781582</v>
-      </c>
-      <c r="L24" s="1">
-        <v>3858118</v>
-      </c>
-      <c r="M24" s="1">
-        <v>3743972</v>
-      </c>
-      <c r="N24" s="1">
-        <v>4204428</v>
-      </c>
-      <c r="O24" s="1">
-        <v>3504428</v>
-      </c>
-      <c r="P24" s="1">
-        <v>3496428</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>3496428</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -2436,32 +1905,8 @@
       <c r="H25">
         <v>6232527</v>
       </c>
-      <c r="J25" t="s">
-        <v>62</v>
-      </c>
-      <c r="K25" s="1">
-        <v>6496735</v>
-      </c>
-      <c r="L25" s="1">
-        <v>8052253</v>
-      </c>
-      <c r="M25" s="1">
-        <v>6861311</v>
-      </c>
-      <c r="N25" s="1">
-        <v>9191713</v>
-      </c>
-      <c r="O25" s="1">
-        <v>9191713</v>
-      </c>
-      <c r="P25" s="1">
-        <v>9191713</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>9191713</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -2486,32 +1931,8 @@
       <c r="H26">
         <v>2453702</v>
       </c>
-      <c r="J26" t="s">
-        <v>63</v>
-      </c>
-      <c r="K26" s="1">
-        <v>835264</v>
-      </c>
-      <c r="L26" s="1">
-        <v>792597</v>
-      </c>
-      <c r="M26" s="1">
-        <v>864531</v>
-      </c>
-      <c r="N26" s="1">
-        <v>851868</v>
-      </c>
-      <c r="O26" s="1">
-        <v>851868</v>
-      </c>
-      <c r="P26" s="1">
-        <v>792500</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>780500</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -2536,32 +1957,8 @@
       <c r="H27">
         <v>2097256</v>
       </c>
-      <c r="J27" t="s">
-        <v>64</v>
-      </c>
-      <c r="K27" s="1">
-        <v>2632711</v>
-      </c>
-      <c r="L27" s="1">
-        <v>2237128</v>
-      </c>
-      <c r="M27" s="1">
-        <v>2193961</v>
-      </c>
-      <c r="N27" s="1">
-        <v>2086780</v>
-      </c>
-      <c r="O27" s="1">
-        <v>2111455</v>
-      </c>
-      <c r="P27" s="1">
-        <v>3043752</v>
-      </c>
-      <c r="Q27" s="1">
-        <v>3056813</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2586,34 +1983,8 @@
       <c r="H28">
         <v>5741525</v>
       </c>
-      <c r="J28" t="s">
-        <v>104</v>
-      </c>
-      <c r="K28" s="1">
-        <v>78447536</v>
-      </c>
-      <c r="L28" s="1">
-        <v>84757533</v>
-      </c>
-      <c r="M28" s="1">
-        <v>84855130</v>
-      </c>
-      <c r="N28" s="1">
-        <v>87029366</v>
-      </c>
-      <c r="O28" s="1">
-        <v>86777919</v>
-      </c>
-      <c r="P28" s="1">
-        <f>SUM(P18:P27)</f>
-        <v>101765611</v>
-      </c>
-      <c r="Q28" s="1">
-        <f>SUM(Q18:Q27)</f>
-        <v>104480731</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2638,13 +2009,8 @@
       <c r="H29">
         <v>2024979</v>
       </c>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2669,32 +2035,8 @@
       <c r="H30">
         <v>14946689</v>
       </c>
-      <c r="J30" t="s">
-        <v>65</v>
-      </c>
-      <c r="K30" s="1">
-        <v>7360154</v>
-      </c>
-      <c r="L30" s="1">
-        <v>6713733</v>
-      </c>
-      <c r="M30" s="1">
-        <v>6161504</v>
-      </c>
-      <c r="N30" s="1">
-        <v>6042504</v>
-      </c>
-      <c r="O30" s="1">
-        <v>6042504</v>
-      </c>
-      <c r="P30" s="1">
-        <v>9197989</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>9376698</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2719,13 +2061,8 @@
       <c r="H31">
         <v>63187683</v>
       </c>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2750,16 +2087,8 @@
       <c r="H32">
         <v>31985365</v>
       </c>
-      <c r="J32" t="s">
-        <v>66</v>
-      </c>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -2784,32 +2113,8 @@
       <c r="H33">
         <v>3317370</v>
       </c>
-      <c r="J33" t="s">
-        <v>67</v>
-      </c>
-      <c r="K33" s="1">
-        <v>17486</v>
-      </c>
-      <c r="L33" s="1">
-        <v>2639</v>
-      </c>
-      <c r="M33" s="1">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P33" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -2834,32 +2139,8 @@
       <c r="H34">
         <v>5741567</v>
       </c>
-      <c r="J34" t="s">
-        <v>68</v>
-      </c>
-      <c r="K34" s="1">
-        <v>3253</v>
-      </c>
-      <c r="L34" s="1">
-        <v>1032</v>
-      </c>
-      <c r="M34" s="1">
-        <v>0</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P34" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -2884,32 +2165,8 @@
       <c r="H35">
         <v>1939915</v>
       </c>
-      <c r="J35" t="s">
-        <v>69</v>
-      </c>
-      <c r="K35" s="1">
-        <v>0</v>
-      </c>
-      <c r="L35" s="1">
-        <v>14975000</v>
-      </c>
-      <c r="M35" s="1">
-        <v>0</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -2934,32 +2191,8 @@
       <c r="H36">
         <v>6595869</v>
       </c>
-      <c r="J36" t="s">
-        <v>70</v>
-      </c>
-      <c r="K36" s="1">
-        <v>952</v>
-      </c>
-      <c r="L36" s="1">
-        <v>292</v>
-      </c>
-      <c r="M36" s="1">
-        <v>0</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -2984,32 +2217,8 @@
       <c r="H37">
         <v>15265959</v>
       </c>
-      <c r="J37" t="s">
-        <v>71</v>
-      </c>
-      <c r="K37" s="1">
-        <v>0</v>
-      </c>
-      <c r="L37" s="1">
-        <v>0</v>
-      </c>
-      <c r="M37" s="1">
-        <v>103336</v>
-      </c>
-      <c r="N37" s="1">
-        <v>103336</v>
-      </c>
-      <c r="O37" s="1">
-        <v>103336</v>
-      </c>
-      <c r="P37" s="1">
-        <v>103336</v>
-      </c>
-      <c r="Q37" s="1">
-        <v>103336</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -3036,80 +2245,8 @@
         <f>SUM(H20:H37)</f>
         <v>175314252</v>
       </c>
-      <c r="J38" t="s">
-        <v>72</v>
-      </c>
-      <c r="K38" s="1">
-        <v>100002</v>
-      </c>
-      <c r="L38" s="1">
-        <v>100000</v>
-      </c>
-      <c r="M38" s="1">
-        <v>100000</v>
-      </c>
-      <c r="N38" s="1">
-        <v>100000</v>
-      </c>
-      <c r="O38" s="1">
-        <v>100000</v>
-      </c>
-      <c r="P38" s="1">
-        <v>100000</v>
-      </c>
-      <c r="Q38" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J39" t="s">
-        <v>73</v>
-      </c>
-      <c r="K39" s="1">
-        <v>13</v>
-      </c>
-      <c r="L39" s="1">
-        <v>4</v>
-      </c>
-      <c r="M39" s="1">
-        <v>0</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J40" t="s">
-        <v>104</v>
-      </c>
-      <c r="K40" s="1">
-        <v>121706</v>
-      </c>
-      <c r="L40" s="1">
-        <v>15078967</v>
-      </c>
-      <c r="M40" s="1">
-        <v>203336</v>
-      </c>
-      <c r="N40" s="1">
-        <v>203336</v>
-      </c>
-      <c r="O40" s="1">
-        <v>203336</v>
-      </c>
-      <c r="P40" s="1">
-        <f>SUM(P37:P38)</f>
-        <v>203336</v>
-      </c>
-      <c r="Q40" s="1">
-        <f>SUM(Q37:Q38)</f>
-        <v>203336</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>103</v>
       </c>
@@ -3134,13 +2271,8 @@
       <c r="H41" t="s">
         <v>110</v>
       </c>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -3165,16 +2297,8 @@
       <c r="H42">
         <v>2074738</v>
       </c>
-      <c r="J42" t="s">
-        <v>74</v>
-      </c>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -3199,32 +2323,8 @@
       <c r="H43">
         <v>2470998</v>
       </c>
-      <c r="J43" t="s">
-        <v>75</v>
-      </c>
-      <c r="K43" s="1">
-        <v>473295</v>
-      </c>
-      <c r="L43" s="1">
-        <v>473287</v>
-      </c>
-      <c r="M43" s="1">
-        <v>376750</v>
-      </c>
-      <c r="N43" s="1">
-        <v>335750</v>
-      </c>
-      <c r="O43" s="1">
-        <v>296000</v>
-      </c>
-      <c r="P43" s="1">
-        <v>262500</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -3249,32 +2349,8 @@
       <c r="H44">
         <v>738060</v>
       </c>
-      <c r="J44" t="s">
-        <v>76</v>
-      </c>
-      <c r="K44" s="1">
-        <v>1654837</v>
-      </c>
-      <c r="L44" s="1">
-        <v>1752087</v>
-      </c>
-      <c r="M44" s="1">
-        <v>1604969</v>
-      </c>
-      <c r="N44" s="1">
-        <v>1604969</v>
-      </c>
-      <c r="O44" s="1">
-        <v>1604969</v>
-      </c>
-      <c r="P44" s="1">
-        <v>1604969</v>
-      </c>
-      <c r="Q44" s="1">
-        <v>1604969</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -3299,32 +2375,8 @@
       <c r="H45">
         <v>6867862</v>
       </c>
-      <c r="J45" t="s">
-        <v>77</v>
-      </c>
-      <c r="K45" s="1">
-        <v>5829505</v>
-      </c>
-      <c r="L45" s="1">
-        <v>456963</v>
-      </c>
-      <c r="M45" s="1">
-        <v>500317</v>
-      </c>
-      <c r="N45" s="1">
-        <v>500645</v>
-      </c>
-      <c r="O45" s="1">
-        <v>499333</v>
-      </c>
-      <c r="P45" s="1">
-        <v>499942</v>
-      </c>
-      <c r="Q45" s="1">
-        <v>498935</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -3349,32 +2401,8 @@
       <c r="H46">
         <v>5501089</v>
       </c>
-      <c r="J46" t="s">
-        <v>78</v>
-      </c>
-      <c r="K46" s="1">
-        <v>992638</v>
-      </c>
-      <c r="L46" s="1">
-        <v>991639</v>
-      </c>
-      <c r="M46" s="1">
-        <v>0</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P46" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q46" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -3399,32 +2427,8 @@
       <c r="H47">
         <v>17243481</v>
       </c>
-      <c r="J47" t="s">
-        <v>79</v>
-      </c>
-      <c r="K47" s="1">
-        <v>1505385</v>
-      </c>
-      <c r="L47" s="1">
-        <v>1650360</v>
-      </c>
-      <c r="M47" s="1">
-        <v>1463321</v>
-      </c>
-      <c r="N47" s="1">
-        <v>1463321</v>
-      </c>
-      <c r="O47" s="1">
-        <v>1463321</v>
-      </c>
-      <c r="P47" s="1">
-        <v>1463321</v>
-      </c>
-      <c r="Q47" s="1">
-        <v>1463321</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -3449,32 +2453,8 @@
       <c r="H48">
         <v>4418951</v>
       </c>
-      <c r="J48" t="s">
-        <v>80</v>
-      </c>
-      <c r="K48" s="1">
-        <v>3973698</v>
-      </c>
-      <c r="L48" s="1">
-        <v>5321667</v>
-      </c>
-      <c r="M48" s="1">
-        <v>4283772</v>
-      </c>
-      <c r="N48" s="1">
-        <v>4274566</v>
-      </c>
-      <c r="O48" s="1">
-        <v>4280141</v>
-      </c>
-      <c r="P48" s="1">
-        <v>4275466</v>
-      </c>
-      <c r="Q48" s="1">
-        <v>4275416</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -3499,34 +2479,8 @@
       <c r="H49">
         <v>2097256</v>
       </c>
-      <c r="J49" t="s">
-        <v>104</v>
-      </c>
-      <c r="K49" s="1">
-        <v>14429358</v>
-      </c>
-      <c r="L49" s="1">
-        <v>10646003</v>
-      </c>
-      <c r="M49" s="1">
-        <v>8229129</v>
-      </c>
-      <c r="N49" s="1">
-        <v>8179251</v>
-      </c>
-      <c r="O49" s="1">
-        <v>8143764</v>
-      </c>
-      <c r="P49" s="1">
-        <f>SUM(P43:P48)</f>
-        <v>8106198</v>
-      </c>
-      <c r="Q49" s="1">
-        <f>SUM(Q43:Q48)</f>
-        <v>7842641</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -3551,13 +2505,8 @@
       <c r="H50">
         <v>7743231</v>
       </c>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -3582,16 +2531,8 @@
       <c r="H51">
         <v>3900907</v>
       </c>
-      <c r="J51" t="s">
-        <v>81</v>
-      </c>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -3616,32 +2557,8 @@
       <c r="H52">
         <v>48602035</v>
       </c>
-      <c r="J52" t="s">
-        <v>82</v>
-      </c>
-      <c r="K52" s="1">
-        <v>7320500</v>
-      </c>
-      <c r="L52" s="1">
-        <v>8012853</v>
-      </c>
-      <c r="M52" s="1">
-        <v>7274894</v>
-      </c>
-      <c r="N52" s="1">
-        <v>7559973</v>
-      </c>
-      <c r="O52" s="1">
-        <v>7559973</v>
-      </c>
-      <c r="P52" s="1">
-        <v>9810018</v>
-      </c>
-      <c r="Q52" s="1">
-        <v>9810018</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -3666,32 +2583,8 @@
       <c r="H53">
         <v>68665330</v>
       </c>
-      <c r="J53" t="s">
-        <v>83</v>
-      </c>
-      <c r="K53" s="1">
-        <v>20919526</v>
-      </c>
-      <c r="L53" s="1">
-        <v>22821757</v>
-      </c>
-      <c r="M53" s="1">
-        <v>18303336</v>
-      </c>
-      <c r="N53" s="1">
-        <v>19965975</v>
-      </c>
-      <c r="O53" s="1">
-        <v>19859520</v>
-      </c>
-      <c r="P53" s="1">
-        <v>19257523</v>
-      </c>
-      <c r="Q53" s="1">
-        <v>19507523</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -3716,32 +2609,8 @@
       <c r="H54">
         <v>40213292</v>
       </c>
-      <c r="J54" t="s">
-        <v>84</v>
-      </c>
-      <c r="K54" s="1">
-        <v>580696</v>
-      </c>
-      <c r="L54" s="1">
-        <v>255002</v>
-      </c>
-      <c r="M54" s="1">
-        <v>207762</v>
-      </c>
-      <c r="N54" s="1">
-        <v>330962</v>
-      </c>
-      <c r="O54" s="1">
-        <v>330962</v>
-      </c>
-      <c r="P54" s="1">
-        <v>263447</v>
-      </c>
-      <c r="Q54" s="1">
-        <v>263447</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -3766,34 +2635,8 @@
       <c r="H55">
         <v>115099741</v>
       </c>
-      <c r="J55" t="s">
-        <v>104</v>
-      </c>
-      <c r="K55" s="1">
-        <v>28820722</v>
-      </c>
-      <c r="L55" s="1">
-        <v>31089612</v>
-      </c>
-      <c r="M55" s="1">
-        <v>25785992</v>
-      </c>
-      <c r="N55" s="1">
-        <v>27856910</v>
-      </c>
-      <c r="O55" s="1">
-        <v>27750455</v>
-      </c>
-      <c r="P55" s="1">
-        <f>SUM(P52:P54)</f>
-        <v>29330988</v>
-      </c>
-      <c r="Q55" s="1">
-        <f>SUM(Q52:Q54)</f>
-        <v>29580988</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -3818,13 +2661,8 @@
       <c r="H56">
         <v>26964125</v>
       </c>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -3849,16 +2687,8 @@
       <c r="H57">
         <v>18391816</v>
       </c>
-      <c r="J57" t="s">
-        <v>85</v>
-      </c>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>96</v>
       </c>
@@ -3883,32 +2713,8 @@
       <c r="H58">
         <v>19588394</v>
       </c>
-      <c r="J58" t="s">
-        <v>86</v>
-      </c>
-      <c r="K58" s="1">
-        <v>500000</v>
-      </c>
-      <c r="L58" s="1">
-        <v>500000</v>
-      </c>
-      <c r="M58" s="1">
-        <v>500000</v>
-      </c>
-      <c r="N58" s="1">
-        <v>500000</v>
-      </c>
-      <c r="O58" s="1">
-        <v>500000</v>
-      </c>
-      <c r="P58" s="1">
-        <v>750000</v>
-      </c>
-      <c r="Q58" s="1">
-        <v>750000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>97</v>
       </c>
@@ -3933,32 +2739,8 @@
       <c r="H59">
         <v>5525740</v>
       </c>
-      <c r="J59" t="s">
-        <v>87</v>
-      </c>
-      <c r="K59" s="1">
-        <v>4472629</v>
-      </c>
-      <c r="L59" s="1">
-        <v>3560595</v>
-      </c>
-      <c r="M59" s="1">
-        <v>3743406</v>
-      </c>
-      <c r="N59" s="1">
-        <v>4023406</v>
-      </c>
-      <c r="O59" s="1">
-        <v>4023406</v>
-      </c>
-      <c r="P59" s="1">
-        <v>4163406</v>
-      </c>
-      <c r="Q59" s="1">
-        <v>4163406</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -3983,32 +2765,8 @@
       <c r="H60">
         <v>45508051</v>
       </c>
-      <c r="J60" t="s">
-        <v>88</v>
-      </c>
-      <c r="K60" s="1">
-        <v>7474062</v>
-      </c>
-      <c r="L60" s="1">
-        <v>6910069</v>
-      </c>
-      <c r="M60" s="1">
-        <v>6461013</v>
-      </c>
-      <c r="N60" s="1">
-        <v>6461013</v>
-      </c>
-      <c r="O60" s="1">
-        <v>6461013</v>
-      </c>
-      <c r="P60" s="1">
-        <v>6461013</v>
-      </c>
-      <c r="Q60" s="1">
-        <v>6461013</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>104</v>
       </c>
@@ -4035,32 +2793,8 @@
         <f>SUM(H42:H60)</f>
         <v>441615097</v>
       </c>
-      <c r="J61" t="s">
-        <v>89</v>
-      </c>
-      <c r="K61" s="1">
-        <v>3616367</v>
-      </c>
-      <c r="L61" s="1">
-        <v>3573407</v>
-      </c>
-      <c r="M61" s="1">
-        <v>3588738</v>
-      </c>
-      <c r="N61" s="1">
-        <v>3588738</v>
-      </c>
-      <c r="O61" s="1">
-        <v>3588738</v>
-      </c>
-      <c r="P61" s="1">
-        <v>3588738</v>
-      </c>
-      <c r="Q61" s="1">
-        <v>3588738</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -4085,32 +2819,8 @@
       <c r="H62" t="s">
         <v>101</v>
       </c>
-      <c r="J62" t="s">
-        <v>90</v>
-      </c>
-      <c r="K62" s="1">
-        <v>325824</v>
-      </c>
-      <c r="L62" s="1">
-        <v>327822</v>
-      </c>
-      <c r="M62" s="1">
-        <v>225000</v>
-      </c>
-      <c r="N62" s="1">
-        <v>225000</v>
-      </c>
-      <c r="O62" s="1">
-        <v>225000</v>
-      </c>
-      <c r="P62" s="1">
-        <v>225000</v>
-      </c>
-      <c r="Q62" s="1">
-        <v>225000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -4135,32 +2845,8 @@
       <c r="H63">
         <v>-25157694</v>
       </c>
-      <c r="J63" t="s">
-        <v>91</v>
-      </c>
-      <c r="K63" s="1">
-        <v>380826</v>
-      </c>
-      <c r="L63" s="1">
-        <v>384216</v>
-      </c>
-      <c r="M63" s="1">
-        <v>382998</v>
-      </c>
-      <c r="N63" s="1">
-        <v>382998</v>
-      </c>
-      <c r="O63" s="1">
-        <v>382998</v>
-      </c>
-      <c r="P63" s="1">
-        <v>382998</v>
-      </c>
-      <c r="Q63" s="1">
-        <v>382998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -4187,1020 +2873,2454 @@
         <f>SUM(H63,H42:H60)</f>
         <v>416457403</v>
       </c>
-      <c r="J64" t="s">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" t="s">
+        <v>23</v>
+      </c>
+      <c r="F66" t="s">
+        <v>24</v>
+      </c>
+      <c r="G66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" s="1">
+        <v>984051</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1032227</v>
+      </c>
+      <c r="D68" s="1">
+        <v>1052122</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1070929</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1092347</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1209625</v>
+      </c>
+      <c r="H68" s="1">
+        <v>1233817</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" s="1">
+        <v>3110933</v>
+      </c>
+      <c r="C69" s="1">
+        <v>3226626</v>
+      </c>
+      <c r="D69" s="1">
+        <v>2844356</v>
+      </c>
+      <c r="E69" s="1">
+        <v>3050030</v>
+      </c>
+      <c r="F69" s="1">
+        <v>3191390</v>
+      </c>
+      <c r="G69" s="1">
+        <v>3417084</v>
+      </c>
+      <c r="H69" s="1">
+        <v>3475415</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70" s="1">
+        <v>9542084</v>
+      </c>
+      <c r="C70" s="1">
+        <v>9762684</v>
+      </c>
+      <c r="D70" s="1">
+        <v>9948439</v>
+      </c>
+      <c r="E70" s="1">
+        <v>11826449</v>
+      </c>
+      <c r="F70" s="1">
+        <v>12027328</v>
+      </c>
+      <c r="G70" s="1">
+        <v>12816390</v>
+      </c>
+      <c r="H70" s="1">
+        <v>13081657</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71" s="1">
+        <v>969769</v>
+      </c>
+      <c r="C71" s="1">
+        <v>947947</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1005000</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1005000</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1005000</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1250000</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1250000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72" s="1">
+        <v>3917791</v>
+      </c>
+      <c r="C72" s="1">
+        <v>4130013</v>
+      </c>
+      <c r="D72" s="1">
+        <v>4186198</v>
+      </c>
+      <c r="E72" s="1">
+        <v>4256305</v>
+      </c>
+      <c r="F72" s="1">
+        <v>4341432</v>
+      </c>
+      <c r="G72" s="1">
+        <v>4812892</v>
+      </c>
+      <c r="H72" s="1">
+        <v>4909150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2052466</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2065845</v>
+      </c>
+      <c r="D73" s="1">
+        <v>2023244</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1866961</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1866961</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1352432</v>
+      </c>
+      <c r="H73" s="1">
+        <v>1410489</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="1">
+        <v>52888</v>
+      </c>
+      <c r="C74" s="1">
+        <v>28164</v>
+      </c>
+      <c r="D74" s="1">
+        <v>35000</v>
+      </c>
+      <c r="E74" s="1">
+        <v>35000</v>
+      </c>
+      <c r="F74" s="1">
+        <v>35000</v>
+      </c>
+      <c r="G74" s="1">
+        <v>35000</v>
+      </c>
+      <c r="H74" s="1">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>49</v>
+      </c>
+      <c r="B75" s="1">
+        <v>4613</v>
+      </c>
+      <c r="C75" s="1">
+        <v>10</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" s="1">
+        <v>226933</v>
+      </c>
+      <c r="C76" s="1">
+        <v>226450</v>
+      </c>
+      <c r="D76" s="1">
+        <v>263000</v>
+      </c>
+      <c r="E76" s="1">
+        <v>263000</v>
+      </c>
+      <c r="F76" s="1">
+        <v>263000</v>
+      </c>
+      <c r="G76" s="1">
+        <v>489000</v>
+      </c>
+      <c r="H76" s="1">
+        <v>489000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>51</v>
+      </c>
+      <c r="B77" s="1">
+        <v>165672</v>
+      </c>
+      <c r="C77" s="1">
+        <v>164558</v>
+      </c>
+      <c r="D77" s="1">
+        <v>168550</v>
+      </c>
+      <c r="E77" s="1">
+        <v>168550</v>
+      </c>
+      <c r="F77" s="1">
+        <v>168550</v>
+      </c>
+      <c r="G77" s="1">
+        <v>174011</v>
+      </c>
+      <c r="H77" s="1">
+        <v>174011</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>488864</v>
+      </c>
+      <c r="D78" s="1">
+        <v>496424</v>
+      </c>
+      <c r="E78" s="1">
+        <v>546823</v>
+      </c>
+      <c r="F78" s="1">
+        <v>557759</v>
+      </c>
+      <c r="G78" s="1">
+        <v>664136</v>
+      </c>
+      <c r="H78" s="1">
+        <v>674098</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0</v>
+      </c>
+      <c r="D79" s="1">
+        <v>30000</v>
+      </c>
+      <c r="E79" s="1">
+        <v>30000</v>
+      </c>
+      <c r="F79" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G79" s="1">
+        <v>30000</v>
+      </c>
+      <c r="H79" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="1">
+        <v>21027200</v>
+      </c>
+      <c r="C80" s="1">
+        <v>22073388</v>
+      </c>
+      <c r="D80" s="1">
+        <v>22052333</v>
+      </c>
+      <c r="E80" s="1">
+        <v>24119047</v>
+      </c>
+      <c r="F80" s="1">
+        <v>24578767</v>
+      </c>
+      <c r="G80" s="1">
+        <f>SUM(G68:G79)</f>
+        <v>26250570</v>
+      </c>
+      <c r="H80" s="1">
+        <f>SUM(H68:H79)</f>
+        <v>26762637</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>54</v>
+      </c>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>55</v>
+      </c>
+      <c r="B83" s="1">
+        <v>33861186</v>
+      </c>
+      <c r="C83" s="1">
+        <v>34101574</v>
+      </c>
+      <c r="D83" s="1">
+        <v>36673523</v>
+      </c>
+      <c r="E83" s="1">
+        <v>37600783</v>
+      </c>
+      <c r="F83" s="1">
+        <v>37710238</v>
+      </c>
+      <c r="G83" s="1">
+        <v>40453300</v>
+      </c>
+      <c r="H83" s="1">
+        <v>41242753</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>56</v>
+      </c>
+      <c r="B84" s="1">
+        <v>5230735</v>
+      </c>
+      <c r="C84" s="1">
+        <v>5478724</v>
+      </c>
+      <c r="D84" s="1">
+        <v>5558716</v>
+      </c>
+      <c r="E84" s="1">
+        <v>5311066</v>
+      </c>
+      <c r="F84" s="1">
+        <v>5311066</v>
+      </c>
+      <c r="G84" s="1">
+        <v>6245459</v>
+      </c>
+      <c r="H84" s="1">
+        <v>6270459</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>57</v>
+      </c>
+      <c r="B85" s="1">
+        <v>13315067</v>
+      </c>
+      <c r="C85" s="1">
+        <v>13588024</v>
+      </c>
+      <c r="D85" s="1">
+        <v>12801227</v>
+      </c>
+      <c r="E85" s="1">
+        <v>12801227</v>
+      </c>
+      <c r="F85" s="1">
+        <v>12801227</v>
+      </c>
+      <c r="G85" s="1">
+        <v>21384982</v>
+      </c>
+      <c r="H85" s="1">
+        <v>22827768</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>58</v>
+      </c>
+      <c r="B86" s="1">
+        <v>2467033</v>
+      </c>
+      <c r="C86" s="1">
+        <v>2316216</v>
+      </c>
+      <c r="D86" s="1">
+        <v>2365140</v>
+      </c>
+      <c r="E86" s="1">
+        <v>2502740</v>
+      </c>
+      <c r="F86" s="1">
+        <v>2510569</v>
+      </c>
+      <c r="G86" s="1">
+        <v>2388633</v>
+      </c>
+      <c r="H86" s="1">
+        <v>2369937</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>59</v>
+      </c>
+      <c r="B87" s="1">
+        <v>577473</v>
+      </c>
+      <c r="C87" s="1">
+        <v>245868</v>
+      </c>
+      <c r="D87" s="1">
+        <v>240501</v>
+      </c>
+      <c r="E87" s="1">
+        <v>240501</v>
+      </c>
+      <c r="F87" s="1">
+        <v>240501</v>
+      </c>
+      <c r="G87" s="1">
+        <v>240501</v>
+      </c>
+      <c r="H87" s="1">
+        <v>240501</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>60</v>
+      </c>
+      <c r="B88" s="1">
+        <v>9249750</v>
+      </c>
+      <c r="C88" s="1">
+        <v>14087031</v>
+      </c>
+      <c r="D88" s="1">
+        <v>13552248</v>
+      </c>
+      <c r="E88" s="1">
+        <v>12238260</v>
+      </c>
+      <c r="F88" s="1">
+        <v>12544854</v>
+      </c>
+      <c r="G88" s="1">
+        <v>14528343</v>
+      </c>
+      <c r="H88" s="1">
+        <v>15003859</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>61</v>
+      </c>
+      <c r="B89" s="1">
+        <v>3781582</v>
+      </c>
+      <c r="C89" s="1">
+        <v>3858118</v>
+      </c>
+      <c r="D89" s="1">
+        <v>3743972</v>
+      </c>
+      <c r="E89" s="1">
+        <v>4204428</v>
+      </c>
+      <c r="F89" s="1">
+        <v>3504428</v>
+      </c>
+      <c r="G89" s="1">
+        <v>3496428</v>
+      </c>
+      <c r="H89" s="1">
+        <v>3496428</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>62</v>
+      </c>
+      <c r="B90" s="1">
+        <v>6496735</v>
+      </c>
+      <c r="C90" s="1">
+        <v>8052253</v>
+      </c>
+      <c r="D90" s="1">
+        <v>6861311</v>
+      </c>
+      <c r="E90" s="1">
+        <v>9191713</v>
+      </c>
+      <c r="F90" s="1">
+        <v>9191713</v>
+      </c>
+      <c r="G90" s="1">
+        <v>9191713</v>
+      </c>
+      <c r="H90" s="1">
+        <v>9191713</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>63</v>
+      </c>
+      <c r="B91" s="1">
+        <v>835264</v>
+      </c>
+      <c r="C91" s="1">
+        <v>792597</v>
+      </c>
+      <c r="D91" s="1">
+        <v>864531</v>
+      </c>
+      <c r="E91" s="1">
+        <v>851868</v>
+      </c>
+      <c r="F91" s="1">
+        <v>851868</v>
+      </c>
+      <c r="G91" s="1">
+        <v>792500</v>
+      </c>
+      <c r="H91" s="1">
+        <v>780500</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>64</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2632711</v>
+      </c>
+      <c r="C92" s="1">
+        <v>2237128</v>
+      </c>
+      <c r="D92" s="1">
+        <v>2193961</v>
+      </c>
+      <c r="E92" s="1">
+        <v>2086780</v>
+      </c>
+      <c r="F92" s="1">
+        <v>2111455</v>
+      </c>
+      <c r="G92" s="1">
+        <v>3043752</v>
+      </c>
+      <c r="H92" s="1">
+        <v>3056813</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" s="1">
+        <v>78447536</v>
+      </c>
+      <c r="C93" s="1">
+        <v>84757533</v>
+      </c>
+      <c r="D93" s="1">
+        <v>84855130</v>
+      </c>
+      <c r="E93" s="1">
+        <v>87029366</v>
+      </c>
+      <c r="F93" s="1">
+        <v>86777919</v>
+      </c>
+      <c r="G93" s="1">
+        <f>SUM(G83:G92)</f>
+        <v>101765611</v>
+      </c>
+      <c r="H93" s="1">
+        <f>SUM(H83:H92)</f>
+        <v>104480731</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" s="1">
+        <v>7360154</v>
+      </c>
+      <c r="C95" s="1">
+        <v>6713733</v>
+      </c>
+      <c r="D95" s="1">
+        <v>6161504</v>
+      </c>
+      <c r="E95" s="1">
+        <v>6042504</v>
+      </c>
+      <c r="F95" s="1">
+        <v>6042504</v>
+      </c>
+      <c r="G95" s="1">
+        <v>9197989</v>
+      </c>
+      <c r="H95" s="1">
+        <v>9376698</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>66</v>
+      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>67</v>
+      </c>
+      <c r="B98" s="1">
+        <v>17486</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2639</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G98" t="s">
+        <v>101</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>68</v>
+      </c>
+      <c r="B99" s="1">
+        <v>3253</v>
+      </c>
+      <c r="C99" s="1">
+        <v>1032</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G99" t="s">
+        <v>101</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>69</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0</v>
+      </c>
+      <c r="C100" s="1">
+        <v>14975000</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>70</v>
+      </c>
+      <c r="B101" s="1">
+        <v>952</v>
+      </c>
+      <c r="C101" s="1">
+        <v>292</v>
+      </c>
+      <c r="D101" s="1">
+        <v>0</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>71</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0</v>
+      </c>
+      <c r="D102" s="1">
+        <v>103336</v>
+      </c>
+      <c r="E102" s="1">
+        <v>103336</v>
+      </c>
+      <c r="F102" s="1">
+        <v>103336</v>
+      </c>
+      <c r="G102" s="1">
+        <v>103336</v>
+      </c>
+      <c r="H102" s="1">
+        <v>103336</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>72</v>
+      </c>
+      <c r="B103" s="1">
+        <v>100002</v>
+      </c>
+      <c r="C103" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D103" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E103" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F103" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G103" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H103" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>73</v>
+      </c>
+      <c r="B104" s="1">
+        <v>13</v>
+      </c>
+      <c r="C104" s="1">
+        <v>4</v>
+      </c>
+      <c r="D104" s="1">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" s="1">
+        <v>121706</v>
+      </c>
+      <c r="C105" s="1">
+        <v>15078967</v>
+      </c>
+      <c r="D105" s="1">
+        <v>203336</v>
+      </c>
+      <c r="E105" s="1">
+        <v>203336</v>
+      </c>
+      <c r="F105" s="1">
+        <v>203336</v>
+      </c>
+      <c r="G105" s="1">
+        <f>SUM(G102:G103)</f>
+        <v>203336</v>
+      </c>
+      <c r="H105" s="1">
+        <f>SUM(H102:H103)</f>
+        <v>203336</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>74</v>
+      </c>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>75</v>
+      </c>
+      <c r="B108" s="1">
+        <v>473295</v>
+      </c>
+      <c r="C108" s="1">
+        <v>473287</v>
+      </c>
+      <c r="D108" s="1">
+        <v>376750</v>
+      </c>
+      <c r="E108" s="1">
+        <v>335750</v>
+      </c>
+      <c r="F108" s="1">
+        <v>296000</v>
+      </c>
+      <c r="G108" s="1">
+        <v>262500</v>
+      </c>
+      <c r="H108" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>76</v>
+      </c>
+      <c r="B109" s="1">
+        <v>1654837</v>
+      </c>
+      <c r="C109" s="1">
+        <v>1752087</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1604969</v>
+      </c>
+      <c r="E109" s="1">
+        <v>1604969</v>
+      </c>
+      <c r="F109" s="1">
+        <v>1604969</v>
+      </c>
+      <c r="G109" s="1">
+        <v>1604969</v>
+      </c>
+      <c r="H109" s="1">
+        <v>1604969</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>77</v>
+      </c>
+      <c r="B110" s="1">
+        <v>5829505</v>
+      </c>
+      <c r="C110" s="1">
+        <v>456963</v>
+      </c>
+      <c r="D110" s="1">
+        <v>500317</v>
+      </c>
+      <c r="E110" s="1">
+        <v>500645</v>
+      </c>
+      <c r="F110" s="1">
+        <v>499333</v>
+      </c>
+      <c r="G110" s="1">
+        <v>499942</v>
+      </c>
+      <c r="H110" s="1">
+        <v>498935</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>78</v>
+      </c>
+      <c r="B111" s="1">
+        <v>992638</v>
+      </c>
+      <c r="C111" s="1">
+        <v>991639</v>
+      </c>
+      <c r="D111" s="1">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G111" t="s">
+        <v>101</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112" s="1">
+        <v>1505385</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1650360</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1463321</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1463321</v>
+      </c>
+      <c r="F112" s="1">
+        <v>1463321</v>
+      </c>
+      <c r="G112" s="1">
+        <v>1463321</v>
+      </c>
+      <c r="H112" s="1">
+        <v>1463321</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>80</v>
+      </c>
+      <c r="B113" s="1">
+        <v>3973698</v>
+      </c>
+      <c r="C113" s="1">
+        <v>5321667</v>
+      </c>
+      <c r="D113" s="1">
+        <v>4283772</v>
+      </c>
+      <c r="E113" s="1">
+        <v>4274566</v>
+      </c>
+      <c r="F113" s="1">
+        <v>4280141</v>
+      </c>
+      <c r="G113" s="1">
+        <v>4275466</v>
+      </c>
+      <c r="H113" s="1">
+        <v>4275416</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>104</v>
+      </c>
+      <c r="B114" s="1">
+        <v>14429358</v>
+      </c>
+      <c r="C114" s="1">
+        <v>10646003</v>
+      </c>
+      <c r="D114" s="1">
+        <v>8229129</v>
+      </c>
+      <c r="E114" s="1">
+        <v>8179251</v>
+      </c>
+      <c r="F114" s="1">
+        <v>8143764</v>
+      </c>
+      <c r="G114" s="1">
+        <f>SUM(G108:G113)</f>
+        <v>8106198</v>
+      </c>
+      <c r="H114" s="1">
+        <f>SUM(H108:H113)</f>
+        <v>7842641</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>81</v>
+      </c>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>82</v>
+      </c>
+      <c r="B117" s="1">
+        <v>7320500</v>
+      </c>
+      <c r="C117" s="1">
+        <v>8012853</v>
+      </c>
+      <c r="D117" s="1">
+        <v>7274894</v>
+      </c>
+      <c r="E117" s="1">
+        <v>7559973</v>
+      </c>
+      <c r="F117" s="1">
+        <v>7559973</v>
+      </c>
+      <c r="G117" s="1">
+        <v>9810018</v>
+      </c>
+      <c r="H117" s="1">
+        <v>9810018</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>83</v>
+      </c>
+      <c r="B118" s="1">
+        <v>20919526</v>
+      </c>
+      <c r="C118" s="1">
+        <v>22821757</v>
+      </c>
+      <c r="D118" s="1">
+        <v>18303336</v>
+      </c>
+      <c r="E118" s="1">
+        <v>19965975</v>
+      </c>
+      <c r="F118" s="1">
+        <v>19859520</v>
+      </c>
+      <c r="G118" s="1">
+        <v>19257523</v>
+      </c>
+      <c r="H118" s="1">
+        <v>19507523</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>84</v>
+      </c>
+      <c r="B119" s="1">
+        <v>580696</v>
+      </c>
+      <c r="C119" s="1">
+        <v>255002</v>
+      </c>
+      <c r="D119" s="1">
+        <v>207762</v>
+      </c>
+      <c r="E119" s="1">
+        <v>330962</v>
+      </c>
+      <c r="F119" s="1">
+        <v>330962</v>
+      </c>
+      <c r="G119" s="1">
+        <v>263447</v>
+      </c>
+      <c r="H119" s="1">
+        <v>263447</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>104</v>
+      </c>
+      <c r="B120" s="1">
+        <v>28820722</v>
+      </c>
+      <c r="C120" s="1">
+        <v>31089612</v>
+      </c>
+      <c r="D120" s="1">
+        <v>25785992</v>
+      </c>
+      <c r="E120" s="1">
+        <v>27856910</v>
+      </c>
+      <c r="F120" s="1">
+        <v>27750455</v>
+      </c>
+      <c r="G120" s="1">
+        <f>SUM(G117:G119)</f>
+        <v>29330988</v>
+      </c>
+      <c r="H120" s="1">
+        <f>SUM(H117:H119)</f>
+        <v>29580988</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>85</v>
+      </c>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>86</v>
+      </c>
+      <c r="B123" s="1">
+        <v>500000</v>
+      </c>
+      <c r="C123" s="1">
+        <v>500000</v>
+      </c>
+      <c r="D123" s="1">
+        <v>500000</v>
+      </c>
+      <c r="E123" s="1">
+        <v>500000</v>
+      </c>
+      <c r="F123" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G123" s="1">
+        <v>750000</v>
+      </c>
+      <c r="H123" s="1">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>87</v>
+      </c>
+      <c r="B124" s="1">
+        <v>4472629</v>
+      </c>
+      <c r="C124" s="1">
+        <v>3560595</v>
+      </c>
+      <c r="D124" s="1">
+        <v>3743406</v>
+      </c>
+      <c r="E124" s="1">
+        <v>4023406</v>
+      </c>
+      <c r="F124" s="1">
+        <v>4023406</v>
+      </c>
+      <c r="G124" s="1">
+        <v>4163406</v>
+      </c>
+      <c r="H124" s="1">
+        <v>4163406</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>88</v>
+      </c>
+      <c r="B125" s="1">
+        <v>7474062</v>
+      </c>
+      <c r="C125" s="1">
+        <v>6910069</v>
+      </c>
+      <c r="D125" s="1">
+        <v>6461013</v>
+      </c>
+      <c r="E125" s="1">
+        <v>6461013</v>
+      </c>
+      <c r="F125" s="1">
+        <v>6461013</v>
+      </c>
+      <c r="G125" s="1">
+        <v>6461013</v>
+      </c>
+      <c r="H125" s="1">
+        <v>6461013</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>89</v>
+      </c>
+      <c r="B126" s="1">
+        <v>3616367</v>
+      </c>
+      <c r="C126" s="1">
+        <v>3573407</v>
+      </c>
+      <c r="D126" s="1">
+        <v>3588738</v>
+      </c>
+      <c r="E126" s="1">
+        <v>3588738</v>
+      </c>
+      <c r="F126" s="1">
+        <v>3588738</v>
+      </c>
+      <c r="G126" s="1">
+        <v>3588738</v>
+      </c>
+      <c r="H126" s="1">
+        <v>3588738</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>90</v>
+      </c>
+      <c r="B127" s="1">
+        <v>325824</v>
+      </c>
+      <c r="C127" s="1">
+        <v>327822</v>
+      </c>
+      <c r="D127" s="1">
+        <v>225000</v>
+      </c>
+      <c r="E127" s="1">
+        <v>225000</v>
+      </c>
+      <c r="F127" s="1">
+        <v>225000</v>
+      </c>
+      <c r="G127" s="1">
+        <v>225000</v>
+      </c>
+      <c r="H127" s="1">
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>91</v>
+      </c>
+      <c r="B128" s="1">
+        <v>380826</v>
+      </c>
+      <c r="C128" s="1">
+        <v>384216</v>
+      </c>
+      <c r="D128" s="1">
+        <v>382998</v>
+      </c>
+      <c r="E128" s="1">
+        <v>382998</v>
+      </c>
+      <c r="F128" s="1">
+        <v>382998</v>
+      </c>
+      <c r="G128" s="1">
+        <v>382998</v>
+      </c>
+      <c r="H128" s="1">
+        <v>382998</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>92</v>
       </c>
-      <c r="K64" s="1">
+      <c r="B129" s="1">
         <v>7967786</v>
       </c>
-      <c r="L64" s="1">
+      <c r="C129" s="1">
         <v>8226975</v>
       </c>
-      <c r="M64" s="1">
+      <c r="D129" s="1">
         <v>8316328</v>
       </c>
-      <c r="N64" s="1">
+      <c r="E129" s="1">
         <v>9199194</v>
       </c>
-      <c r="O64" s="1">
+      <c r="F129" s="1">
         <v>9201683</v>
       </c>
-      <c r="P64" s="1">
+      <c r="G129" s="1">
         <v>9569988</v>
       </c>
-      <c r="Q64" s="1">
+      <c r="H129" s="1">
         <v>9681972</v>
       </c>
     </row>
-    <row r="65" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J65" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>104</v>
       </c>
-      <c r="K65" s="1">
+      <c r="B130" s="1">
         <v>24737494</v>
       </c>
-      <c r="L65" s="1">
+      <c r="C130" s="1">
         <v>23483084</v>
       </c>
-      <c r="M65" s="1">
+      <c r="D130" s="1">
         <v>23217483</v>
       </c>
-      <c r="N65" s="1">
+      <c r="E130" s="1">
         <v>24380349</v>
       </c>
-      <c r="O65" s="1">
+      <c r="F130" s="1">
         <v>24382838</v>
       </c>
-      <c r="P65" s="1">
-        <f>SUM(P58:P64)</f>
+      <c r="G130" s="1">
+        <f>SUM(G123:G129)</f>
         <v>25141143</v>
       </c>
-      <c r="Q65" s="1">
-        <f>SUM(Q58:Q64)</f>
+      <c r="H130" s="1">
+        <f>SUM(H123:H129)</f>
         <v>25253127</v>
       </c>
     </row>
-    <row r="66" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-    </row>
-    <row r="67" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J67" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>93</v>
       </c>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-    </row>
-    <row r="68" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J68" t="s">
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>94</v>
       </c>
-      <c r="K68" s="1">
+      <c r="B133" s="1">
         <v>5305154</v>
       </c>
-      <c r="L68" s="1">
+      <c r="C133" s="1">
         <v>8222193</v>
       </c>
-      <c r="M68" s="1">
+      <c r="D133" s="1">
         <v>7731607</v>
       </c>
-      <c r="N68" s="1">
+      <c r="E133" s="1">
         <v>5501269</v>
       </c>
-      <c r="O68" s="1">
+      <c r="F133" s="1">
         <v>5501269</v>
       </c>
-      <c r="P68" s="1">
+      <c r="G133" s="1">
         <v>5348269</v>
       </c>
-      <c r="Q68" s="1">
+      <c r="H133" s="1">
         <v>5348269</v>
       </c>
     </row>
-    <row r="69" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J69" t="s">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>95</v>
       </c>
-      <c r="K69" s="1">
+      <c r="B134" s="1">
         <v>1752987</v>
       </c>
-      <c r="L69" s="1">
+      <c r="C134" s="1">
         <v>1695888</v>
       </c>
-      <c r="M69" s="1">
+      <c r="D134" s="1">
         <v>1695888</v>
       </c>
-      <c r="N69" s="1">
+      <c r="E134" s="1">
         <v>1695888</v>
       </c>
-      <c r="O69" s="1">
+      <c r="F134" s="1">
         <v>1695888</v>
       </c>
-      <c r="P69" s="1">
+      <c r="G134" s="1">
         <v>695000</v>
       </c>
-      <c r="Q69" s="1">
+      <c r="H134" s="1">
         <v>393623</v>
       </c>
     </row>
-    <row r="70" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J70" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>96</v>
       </c>
-      <c r="K70" s="1">
+      <c r="B135" s="1">
         <v>15488692</v>
       </c>
-      <c r="L70" s="1">
+      <c r="C135" s="1">
         <v>16236039</v>
       </c>
-      <c r="M70" s="1">
+      <c r="D135" s="1">
         <v>16631412</v>
       </c>
-      <c r="N70" s="1">
+      <c r="E135" s="1">
         <v>16904288</v>
       </c>
-      <c r="O70" s="1">
+      <c r="F135" s="1">
         <v>17236634</v>
       </c>
-      <c r="P70" s="1">
+      <c r="G135" s="1">
         <v>19020937</v>
       </c>
-      <c r="Q70" s="1">
+      <c r="H135" s="1">
         <v>19369671</v>
       </c>
     </row>
-    <row r="71" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J71" t="s">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>97</v>
       </c>
-      <c r="K71" s="1">
+      <c r="B136" s="1">
         <v>3911005</v>
       </c>
-      <c r="L71" s="1">
+      <c r="C136" s="1">
         <v>3899835</v>
       </c>
-      <c r="M71" s="1">
+      <c r="D136" s="1">
         <v>3900000</v>
       </c>
-      <c r="N71" s="1">
+      <c r="E136" s="1">
         <v>3900000</v>
       </c>
-      <c r="O71" s="1">
+      <c r="F136" s="1">
         <v>3900000</v>
       </c>
-      <c r="P71" s="1">
+      <c r="G136" s="1">
         <v>5500000</v>
       </c>
-      <c r="Q71" s="1">
+      <c r="H136" s="1">
         <v>5500000</v>
       </c>
     </row>
-    <row r="72" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J72" t="s">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>98</v>
       </c>
-      <c r="K72" s="1">
+      <c r="B137" s="1">
         <v>2746208</v>
       </c>
-      <c r="L72" s="1">
+      <c r="C137" s="1">
         <v>2868432</v>
       </c>
-      <c r="M72" s="1">
+      <c r="D137" s="1">
         <v>3172884</v>
       </c>
-      <c r="N72" s="1">
+      <c r="E137" s="1">
         <v>1222988</v>
       </c>
-      <c r="O72" s="1">
+      <c r="F137" s="1">
         <v>1222988</v>
       </c>
-      <c r="P72" s="1">
+      <c r="G137" s="1">
         <v>486367</v>
       </c>
-      <c r="Q72" s="1">
+      <c r="H137" s="1">
         <v>486367</v>
       </c>
     </row>
-    <row r="73" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J73" t="s">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>99</v>
       </c>
-      <c r="K73" s="1">
+      <c r="B138" s="1">
         <v>2072410</v>
       </c>
-      <c r="L73" s="1">
+      <c r="C138" s="1">
         <v>6352799</v>
       </c>
-      <c r="M73" s="1">
+      <c r="D138" s="1">
         <v>1000832</v>
       </c>
-      <c r="N73" s="1">
+      <c r="E138" s="1">
         <v>1000832</v>
       </c>
-      <c r="O73" s="1">
+      <c r="F138" s="1">
         <v>1000832</v>
       </c>
-      <c r="P73" s="1">
+      <c r="G138" s="1">
         <v>1000832</v>
       </c>
-      <c r="Q73" s="1">
+      <c r="H138" s="1">
         <v>1000832</v>
       </c>
     </row>
-    <row r="74" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J74" t="s">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>100</v>
       </c>
-      <c r="K74" s="1">
+      <c r="B139" s="1">
         <v>3583097</v>
       </c>
-      <c r="L74" s="1">
+      <c r="C139" s="1">
         <v>4081366</v>
       </c>
-      <c r="M74" s="1">
+      <c r="D139" s="1">
         <v>3603018</v>
       </c>
-      <c r="N74" s="1">
+      <c r="E139" s="1">
         <v>3703018</v>
       </c>
-      <c r="O74" s="1">
+      <c r="F139" s="1">
         <v>3703018</v>
       </c>
-      <c r="P74" s="1">
+      <c r="G139" s="1">
         <v>3703018</v>
       </c>
-      <c r="Q74" s="1">
+      <c r="H139" s="1">
         <v>3703018</v>
       </c>
     </row>
-    <row r="75" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J75" t="s">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>93</v>
       </c>
-      <c r="K75" s="1">
+      <c r="B140" s="1">
         <v>5254050</v>
       </c>
-      <c r="L75" s="1">
+      <c r="C140" s="1">
         <v>6405333</v>
       </c>
-      <c r="M75" s="1">
+      <c r="D140" s="1">
         <v>4026059</v>
       </c>
-      <c r="N75" s="1">
+      <c r="E140" s="1">
         <v>4110712</v>
       </c>
-      <c r="O75" s="1">
+      <c r="F140" s="1">
         <v>4176884</v>
       </c>
-      <c r="P75" s="1">
+      <c r="G140" s="1">
         <v>4183079</v>
       </c>
-      <c r="Q75" s="1">
+      <c r="H140" s="1">
         <v>4031843</v>
       </c>
     </row>
-    <row r="76" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J76" t="s">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>104</v>
       </c>
-      <c r="K76" s="1">
+      <c r="B141" s="1">
         <v>40113603</v>
       </c>
-      <c r="L76" s="1">
+      <c r="C141" s="1">
         <v>49761885</v>
       </c>
-      <c r="M76" s="1">
+      <c r="D141" s="1">
         <v>41761700</v>
       </c>
-      <c r="N76" s="1">
+      <c r="E141" s="1">
         <v>38038995</v>
       </c>
-      <c r="O76" s="1">
+      <c r="F141" s="1">
         <v>38437513</v>
       </c>
-      <c r="P76" s="1">
-        <f>SUM(P68:P75)</f>
+      <c r="G141" s="1">
+        <f>SUM(G133:G140)</f>
         <v>39937502</v>
       </c>
-      <c r="Q76" s="1">
-        <f>SUM(Q68:Q75)</f>
+      <c r="H141" s="1">
+        <f>SUM(H133:H140)</f>
         <v>39833623</v>
       </c>
     </row>
-    <row r="77" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-    </row>
-    <row r="78" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J78" t="s">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>102</v>
       </c>
-      <c r="K78" s="1">
+      <c r="B143" s="1">
         <v>215057773</v>
       </c>
-      <c r="L78" s="1">
+      <c r="C143" s="1">
         <v>243604205</v>
       </c>
-      <c r="M78" s="1">
+      <c r="D143" s="1">
         <v>212266607</v>
       </c>
-      <c r="N78" s="1">
+      <c r="E143" s="1">
         <v>215849758</v>
       </c>
-      <c r="O78" s="1">
+      <c r="F143" s="1">
         <v>216317096</v>
       </c>
-      <c r="P78" s="1">
-        <f>SUM(P76,P65,P55,P49,P40,P28,P15)</f>
+      <c r="G143" s="1">
+        <f>SUM(G141,G130,G120,G114,G105,G93,G80)</f>
         <v>230735348</v>
       </c>
-      <c r="Q78" s="1">
-        <f>SUM(Q76,Q65,Q55,Q49,Q40,Q28,Q15)</f>
+      <c r="H143" s="1">
+        <f>SUM(H141,H130,H120,H114,H105,H93,H80)</f>
         <v>233957083</v>
       </c>
     </row>
-    <row r="83" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J83" t="s">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>107</v>
       </c>
-      <c r="K83" t="s">
+      <c r="B148" t="s">
         <v>20</v>
       </c>
-      <c r="L83" t="s">
+      <c r="C148" t="s">
         <v>21</v>
       </c>
-      <c r="M83" t="s">
+      <c r="D148" t="s">
         <v>22</v>
       </c>
-      <c r="N83" t="s">
+      <c r="E148" t="s">
         <v>23</v>
       </c>
-      <c r="O83" t="s">
+      <c r="F148" t="s">
         <v>24</v>
       </c>
-      <c r="P83" t="s">
+      <c r="G148" t="s">
         <v>109</v>
       </c>
-      <c r="Q83" t="s">
+      <c r="H148" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J84" t="s">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>2</v>
       </c>
-      <c r="K84">
+      <c r="B149">
         <v>0</v>
       </c>
-      <c r="L84">
+      <c r="C149">
         <v>0</v>
       </c>
-      <c r="M84">
+      <c r="D149">
         <v>0</v>
       </c>
-      <c r="N84">
+      <c r="E149">
         <v>0</v>
       </c>
-      <c r="O84">
+      <c r="F149">
         <v>0</v>
       </c>
-      <c r="P84">
+      <c r="G149">
         <v>0</v>
       </c>
-      <c r="Q84">
+      <c r="H149">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J85" t="s">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>3</v>
       </c>
-      <c r="K85">
+      <c r="B150">
         <v>119600</v>
       </c>
-      <c r="L85">
+      <c r="C150">
         <v>140132</v>
       </c>
-      <c r="M85">
+      <c r="D150">
         <v>130027</v>
       </c>
-      <c r="N85">
+      <c r="E150">
         <v>153492</v>
       </c>
-      <c r="O85">
+      <c r="F150">
         <v>156260</v>
       </c>
-      <c r="P85">
+      <c r="G150">
         <v>162800</v>
       </c>
-      <c r="Q85">
+      <c r="H150">
         <v>166585</v>
       </c>
     </row>
-    <row r="86" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J86" t="s">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>4</v>
       </c>
-      <c r="K86">
+      <c r="B151">
         <v>0</v>
       </c>
-      <c r="L86">
+      <c r="C151">
         <v>0</v>
       </c>
-      <c r="M86">
+      <c r="D151">
         <v>0</v>
       </c>
-      <c r="N86">
+      <c r="E151">
         <v>0</v>
       </c>
-      <c r="O86">
+      <c r="F151">
         <v>0</v>
       </c>
-      <c r="P86">
+      <c r="G151">
         <v>0</v>
       </c>
-      <c r="Q86">
+      <c r="H151">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J87" t="s">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>5</v>
       </c>
-      <c r="K87">
+      <c r="B152">
         <v>278080</v>
       </c>
-      <c r="L87">
+      <c r="C152">
         <v>272483</v>
       </c>
-      <c r="M87">
+      <c r="D152">
         <v>451961</v>
       </c>
-      <c r="N87">
+      <c r="E152">
         <v>490153</v>
       </c>
-      <c r="O87">
+      <c r="F152">
         <v>494948</v>
       </c>
-      <c r="P87">
+      <c r="G152">
         <f>6637466 - 5883194</f>
         <v>754272</v>
       </c>
-      <c r="Q87">
+      <c r="H152">
         <f>6867862-6106514</f>
         <v>761348</v>
       </c>
     </row>
-    <row r="88" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J88" t="s">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>6</v>
       </c>
-      <c r="K88">
+      <c r="B153">
         <v>1877780</v>
       </c>
-      <c r="L88">
+      <c r="C153">
         <v>1367760</v>
       </c>
-      <c r="M88">
+      <c r="D153">
         <v>2227862</v>
       </c>
-      <c r="N88">
+      <c r="E153">
         <v>2286738</v>
       </c>
-      <c r="O88">
+      <c r="F153">
         <v>2301721</v>
       </c>
-      <c r="P88">
+      <c r="G153">
         <f>5626805-2691403</f>
         <v>2935402</v>
       </c>
-      <c r="Q88">
+      <c r="H153">
         <f>5501089-2560121</f>
         <v>2940968</v>
       </c>
     </row>
-    <row r="89" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J89" t="s">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>7</v>
       </c>
-      <c r="K89">
+      <c r="B154">
         <v>3771757</v>
       </c>
-      <c r="L89">
+      <c r="C154">
         <v>3383853</v>
       </c>
-      <c r="M89">
+      <c r="D154">
         <v>3453425</v>
       </c>
-      <c r="N89">
+      <c r="E154">
         <v>3511390</v>
       </c>
-      <c r="O89">
+      <c r="F154">
         <v>3542616</v>
       </c>
-      <c r="P89">
+      <c r="G154">
         <f>16291888-5770103</f>
         <v>10521785</v>
       </c>
-      <c r="Q89">
+      <c r="H154">
         <f>17243481-6232527</f>
         <v>11010954</v>
       </c>
     </row>
-    <row r="90" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J90" t="s">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>8</v>
       </c>
-      <c r="K90">
+      <c r="B155">
         <v>1229537</v>
       </c>
-      <c r="L90">
+      <c r="C155">
         <v>1696419</v>
       </c>
-      <c r="M90">
+      <c r="D155">
         <v>1719633</v>
       </c>
-      <c r="N90">
+      <c r="E155">
         <v>1776141</v>
       </c>
-      <c r="O90">
+      <c r="F155">
         <v>1784092</v>
       </c>
-      <c r="P90">
+      <c r="G155">
         <f>4343771 - 2398356</f>
         <v>1945415</v>
       </c>
-      <c r="Q90">
+      <c r="H155">
         <f>4418951-2453702</f>
         <v>1965249</v>
       </c>
     </row>
-    <row r="91" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J91" t="s">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>9</v>
       </c>
-      <c r="K91">
+      <c r="B156">
         <v>0</v>
       </c>
-      <c r="L91">
+      <c r="C156">
         <v>0</v>
       </c>
-      <c r="M91">
+      <c r="D156">
         <v>0</v>
       </c>
-      <c r="N91">
+      <c r="E156">
         <v>0</v>
       </c>
-      <c r="O91">
+      <c r="F156">
         <v>0</v>
       </c>
-      <c r="P91">
+      <c r="G156">
         <v>0</v>
       </c>
-      <c r="Q91">
+      <c r="H156">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J92" t="s">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>10</v>
       </c>
-      <c r="K92">
+      <c r="B157">
         <v>1657626</v>
       </c>
-      <c r="L92">
+      <c r="C157">
         <v>1601974</v>
       </c>
-      <c r="M92">
+      <c r="D157">
         <v>1878587</v>
       </c>
-      <c r="N92">
+      <c r="E157">
         <v>1886893</v>
       </c>
-      <c r="O92">
+      <c r="F157">
         <v>1907626</v>
       </c>
-      <c r="P92">
+      <c r="G157">
         <f>7727093-5756160</f>
         <v>1970933</v>
       </c>
-      <c r="Q92">
+      <c r="H157">
         <f>7743231-5741525</f>
         <v>2001706</v>
       </c>
     </row>
-    <row r="93" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J93" t="s">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>11</v>
       </c>
-      <c r="K93">
+      <c r="B158">
         <v>1077991</v>
       </c>
-      <c r="L93">
+      <c r="C158">
         <v>1198629</v>
       </c>
-      <c r="M93">
+      <c r="D158">
         <v>1333418</v>
       </c>
-      <c r="N93">
+      <c r="E158">
         <v>1400864</v>
       </c>
-      <c r="O93">
+      <c r="F158">
         <v>1423561</v>
       </c>
-      <c r="P93">
+      <c r="G158">
         <f>3810616-1977674</f>
         <v>1832942</v>
       </c>
-      <c r="Q93">
+      <c r="H158">
         <f>3900907-2024979</f>
         <v>1875928</v>
       </c>
     </row>
-    <row r="94" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J94" t="s">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>12</v>
       </c>
-      <c r="K94">
+      <c r="B159">
         <v>22732453</v>
       </c>
-      <c r="L94">
+      <c r="C159">
         <v>22956307</v>
       </c>
-      <c r="M94">
+      <c r="D159">
         <v>25490291</v>
       </c>
-      <c r="N94">
+      <c r="E159">
         <v>28954380</v>
       </c>
-      <c r="O94">
+      <c r="F159">
         <v>27580827</v>
       </c>
-      <c r="P94">
+      <c r="G159">
         <f>47355255 - 15049190</f>
         <v>32306065</v>
       </c>
-      <c r="Q94">
+      <c r="H159">
         <f>48602035 - 14946689</f>
         <v>33655346</v>
       </c>
     </row>
-    <row r="95" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J95" t="s">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>13</v>
       </c>
-      <c r="K95">
+      <c r="B160">
         <v>2718030</v>
       </c>
-      <c r="L95">
+      <c r="C160">
         <v>3863903</v>
       </c>
-      <c r="M95">
+      <c r="D160">
         <v>4613303</v>
       </c>
-      <c r="N95">
+      <c r="E160">
         <v>4986922</v>
       </c>
-      <c r="O95">
+      <c r="F160">
         <v>5051999</v>
       </c>
-      <c r="P95">
+      <c r="G160">
         <f>66747004 - 61378677</f>
         <v>5368327</v>
       </c>
-      <c r="Q95">
+      <c r="H160">
         <f>68665330 - 63187683</f>
         <v>5477647</v>
       </c>
     </row>
-    <row r="96" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J96" t="s">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>14</v>
       </c>
-      <c r="K96">
+      <c r="B161">
         <v>5839425</v>
       </c>
-      <c r="L96">
+      <c r="C161">
         <v>5851217</v>
       </c>
-      <c r="M96">
+      <c r="D161">
         <v>7056428</v>
       </c>
-      <c r="N96">
+      <c r="E161">
         <v>7527406</v>
       </c>
-      <c r="O96">
+      <c r="F161">
         <v>7581542</v>
       </c>
-      <c r="P96">
+      <c r="G161">
         <f>39091308-30984535</f>
         <v>8106773</v>
       </c>
-      <c r="Q96">
+      <c r="H161">
         <f>40213292-31985365</f>
         <v>8227927</v>
       </c>
     </row>
-    <row r="97" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J97" t="s">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>15</v>
       </c>
-      <c r="K97">
+      <c r="B162">
         <v>90011682</v>
       </c>
-      <c r="L97">
+      <c r="C162">
         <v>87384742</v>
       </c>
-      <c r="M97">
+      <c r="D162">
         <v>92642275</v>
       </c>
-      <c r="N97">
+      <c r="E162">
         <v>97542225</v>
       </c>
-      <c r="O97">
+      <c r="F162">
         <v>93875848</v>
       </c>
-      <c r="P97">
+      <c r="G162">
         <f>151198065-3276300</f>
         <v>147921765</v>
       </c>
-      <c r="Q97">
+      <c r="H162">
         <f>115099741-317370</f>
         <v>114782371</v>
       </c>
     </row>
-    <row r="98" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J98" t="s">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>16</v>
       </c>
-      <c r="K98">
+      <c r="B163">
         <v>18937891</v>
       </c>
-      <c r="L98">
+      <c r="C163">
         <v>18419202</v>
       </c>
-      <c r="M98">
+      <c r="D163">
         <v>17962391</v>
       </c>
-      <c r="N98">
+      <c r="E163">
         <v>19565560</v>
       </c>
-      <c r="O98">
+      <c r="F163">
         <v>19223958</v>
       </c>
-      <c r="P98">
+      <c r="G163">
         <f>28271481-5389002</f>
         <v>22882479</v>
       </c>
-      <c r="Q98">
+      <c r="H163">
         <f>26964125-5741567</f>
         <v>21222558</v>
       </c>
     </row>
-    <row r="99" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J99" t="s">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
         <v>17</v>
       </c>
-      <c r="K99">
+      <c r="B164">
         <v>9661327</v>
       </c>
-      <c r="L99">
+      <c r="C164">
         <v>10851361</v>
       </c>
-      <c r="M99">
+      <c r="D164">
         <v>11417342</v>
       </c>
-      <c r="N99">
+      <c r="E164">
         <v>12757697</v>
       </c>
-      <c r="O99">
+      <c r="F164">
         <v>12920482</v>
       </c>
-      <c r="P99">
+      <c r="G164">
         <f>18201442-1923055</f>
         <v>16278387</v>
       </c>
-      <c r="Q99">
+      <c r="H164">
         <f>18391816 - 1939915</f>
         <v>16451901</v>
       </c>
     </row>
-    <row r="100" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J100" t="s">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>96</v>
       </c>
-      <c r="K100">
+      <c r="B165">
         <v>23743956</v>
       </c>
-      <c r="L100">
+      <c r="C165">
         <v>20326538</v>
       </c>
-      <c r="M100">
+      <c r="D165">
         <v>19094157</v>
       </c>
-      <c r="N100">
+      <c r="E165">
         <v>18908184</v>
       </c>
-      <c r="O100">
+      <c r="F165">
         <v>17577785</v>
       </c>
-      <c r="P100">
+      <c r="G165">
         <f>20990466 - 20159016</f>
         <v>831450</v>
       </c>
-      <c r="Q100">
+      <c r="H165">
         <f>19588394-19305833</f>
         <v>282561</v>
       </c>
     </row>
-    <row r="101" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J101" t="s">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>97</v>
       </c>
-      <c r="K101">
+      <c r="B166">
         <v>3985087</v>
       </c>
-      <c r="L101">
+      <c r="C166">
         <v>3826758</v>
       </c>
-      <c r="M101">
+      <c r="D166">
         <v>4245000</v>
       </c>
-      <c r="N101">
+      <c r="E166">
         <v>4476410</v>
       </c>
-      <c r="O101">
+      <c r="F166">
         <v>4528273</v>
       </c>
-      <c r="P101">
+      <c r="G166">
         <v>5525740</v>
       </c>
-      <c r="Q101">
+      <c r="H166">
         <v>5525740</v>
       </c>
     </row>
-    <row r="102" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J102" t="s">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>18</v>
       </c>
-      <c r="K102">
+      <c r="B167">
         <v>0</v>
       </c>
-      <c r="L102">
+      <c r="C167">
         <v>0</v>
       </c>
-      <c r="M102">
+      <c r="D167">
         <v>0</v>
       </c>
-      <c r="N102">
+      <c r="E167">
         <v>0</v>
       </c>
-      <c r="O102">
+      <c r="F167">
         <v>0</v>
       </c>
-      <c r="P102">
+      <c r="G167">
         <v>0</v>
       </c>
-      <c r="Q102">
+      <c r="H167">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J103" t="s">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>19</v>
       </c>
-      <c r="K103">
+      <c r="B168">
         <v>41825076</v>
       </c>
-      <c r="L103">
+      <c r="C168">
         <v>29838712</v>
       </c>
-      <c r="M103">
+      <c r="D168">
         <v>32139517</v>
       </c>
-      <c r="N103">
+      <c r="E168">
         <v>32435139</v>
       </c>
-      <c r="O103">
+      <c r="F168">
         <v>31709537</v>
       </c>
-      <c r="P103">
+      <c r="G168">
         <f>47343920 - 23042703</f>
         <v>24301217</v>
       </c>
-      <c r="Q103">
+      <c r="H168">
         <f>45508051-21861828</f>
         <v>23646223</v>
       </c>
     </row>
-    <row r="104" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J104" t="s">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>104</v>
       </c>
-      <c r="K104">
+      <c r="B169">
         <v>229467298</v>
       </c>
-      <c r="L104">
+      <c r="C169">
         <v>212979990</v>
       </c>
-      <c r="M104">
+      <c r="D169">
         <v>225855617</v>
       </c>
-      <c r="N104">
+      <c r="E169">
         <v>238659594</v>
       </c>
-      <c r="O104">
+      <c r="F169">
         <v>231661075</v>
       </c>
-      <c r="P104">
-        <f>SUM(P84:P103)</f>
+      <c r="G169">
+        <f>SUM(G149:G168)</f>
         <v>283645752</v>
       </c>
-      <c r="Q104">
-        <f>SUM(Q84:Q103)</f>
+      <c r="H169">
+        <f>SUM(H149:H168)</f>
         <v>249995012</v>
       </c>
     </row>
-    <row r="105" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J105" t="s">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>108</v>
       </c>
-      <c r="K105">
+      <c r="B170">
         <v>138374</v>
       </c>
-      <c r="L105">
+      <c r="C170">
         <v>25326</v>
       </c>
-      <c r="M105" s="1" t="s">
+      <c r="D170" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="N105" s="1" t="s">
+      <c r="E170" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O105" s="1" t="s">
+      <c r="F170" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="P105" s="1" t="s">
+      <c r="G170" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Q105" s="1" t="s">
+      <c r="H170" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J106" t="s">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>105</v>
       </c>
-      <c r="M106">
+      <c r="D171">
         <v>-52331726</v>
       </c>
-      <c r="N106">
+      <c r="E171">
         <v>-55258672</v>
       </c>
-      <c r="O106">
+      <c r="F171">
         <v>-54317462</v>
       </c>
-      <c r="P106">
+      <c r="G171">
         <v>-25589992</v>
       </c>
-      <c r="Q106">
+      <c r="H171">
         <v>-25157694</v>
       </c>
     </row>
-    <row r="107" spans="10:17" x14ac:dyDescent="0.2">
-      <c r="J107" t="s">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>106</v>
       </c>
-      <c r="K107">
+      <c r="B172">
         <v>229467298</v>
       </c>
-      <c r="L107">
+      <c r="C172">
         <v>212979990</v>
       </c>
-      <c r="M107">
+      <c r="D172">
         <v>173523891</v>
       </c>
-      <c r="N107">
+      <c r="E172">
         <v>183400922</v>
       </c>
-      <c r="O107">
+      <c r="F172">
         <v>177343613</v>
       </c>
-      <c r="P107">
-        <f>SUM(P106,P104)</f>
+      <c r="G172">
+        <f>SUM(G171,G169)</f>
         <v>258055760</v>
       </c>
-      <c r="Q107">
-        <f>SUM(Q106,Q104)</f>
+      <c r="H172">
+        <f>SUM(H171,H169)</f>
         <v>224837318</v>
       </c>
     </row>

</xml_diff>